<commit_message>
-Added calculation for Catch - calculate the root(in the interval [-1,1]) to the actual value(in the interval[a,b] -Added some code to the sgp4 python file
</commit_message>
<xml_diff>
--- a/Test Data/test.xlsx
+++ b/Test Data/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halel\Desktop\פרויקט גמר\Project\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halel\Desktop\פרויקט גמר\test\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E95D58D-874F-4343-8565-7FB749E0EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B175C9-B1ED-47DC-ACFC-4418597C94CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>r1x</t>
   </si>
@@ -135,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,16 +144,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -172,18 +192,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="1" builtinId="10"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -461,13 +485,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE44"/>
+  <dimension ref="A1:AE54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:A42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1682,30 +1709,30 @@
       <c r="O14">
         <v>5893.5407290000003</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="2">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="2">
         <v>2540.7465990000001</v>
       </c>
-      <c r="U14" s="1">
+      <c r="U14" s="2">
         <f t="shared" si="1"/>
         <v>443.66045500000018</v>
       </c>
-      <c r="V14" s="1">
+      <c r="V14" s="2">
         <f t="shared" si="2"/>
         <v>214.36265999999978</v>
       </c>
-      <c r="W14" s="1">
+      <c r="W14" s="2">
         <f t="shared" si="3"/>
         <v>119.85848899999996</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="2">
         <f t="shared" si="4"/>
         <v>257152.00671844583</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Y14" s="2">
         <f t="shared" si="5"/>
         <v>507.10157436005443</v>
       </c>
@@ -3143,48 +3170,48 @@
       <c r="M40">
         <v>-5.3251580430000001</v>
       </c>
-      <c r="S40" s="2">
+      <c r="S40" s="3">
         <f t="shared" si="18"/>
         <v>13</v>
       </c>
-      <c r="T40" s="2">
+      <c r="T40" s="3">
         <v>2106.7352660000001</v>
       </c>
-      <c r="U40" s="2">
+      <c r="U40" s="3">
         <f t="shared" si="11"/>
         <v>-1348.9359050000003</v>
       </c>
-      <c r="V40" s="2">
+      <c r="V40" s="3">
         <f t="shared" si="12"/>
         <v>1418.8999930000009</v>
       </c>
-      <c r="W40" s="2">
+      <c r="W40" s="3">
         <f t="shared" si="13"/>
         <v>-5902.8642139999993</v>
       </c>
-      <c r="X40" s="2">
+      <c r="X40" s="3">
         <f t="shared" si="14"/>
         <v>38676711.194855399</v>
       </c>
-      <c r="Y40" s="2">
+      <c r="Y40" s="3">
         <f t="shared" si="15"/>
         <v>6219.0603144571123</v>
       </c>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AB40" s="2">
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3">
         <f t="shared" si="16"/>
         <v>3.9221611049999998</v>
       </c>
-      <c r="AC40" s="2">
+      <c r="AC40" s="3">
         <f t="shared" si="9"/>
         <v>-2.4919725489999998</v>
       </c>
-      <c r="AD40" s="2">
+      <c r="AD40" s="3">
         <f t="shared" si="10"/>
         <v>12.803499988999999</v>
       </c>
-      <c r="AE40" s="2">
+      <c r="AE40" s="3">
         <f t="shared" si="17"/>
         <v>-168807.85134215749</v>
       </c>
@@ -3229,48 +3256,48 @@
       <c r="M41">
         <v>-6.2738362280000004</v>
       </c>
-      <c r="S41" s="2">
+      <c r="S41" s="3">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="T41" s="2">
+      <c r="T41" s="3">
         <v>2282.2965380000001</v>
       </c>
-      <c r="U41" s="2">
+      <c r="U41" s="3">
         <f t="shared" si="11"/>
         <v>-638.78230500000018</v>
       </c>
-      <c r="V41" s="2">
+      <c r="V41" s="3">
         <f t="shared" si="12"/>
         <v>956.79749300000003</v>
       </c>
-      <c r="W41" s="2">
+      <c r="W41" s="3">
         <f t="shared" si="13"/>
         <v>-3556.1470386999999</v>
       </c>
-      <c r="X41" s="2">
+      <c r="X41" s="3">
         <f t="shared" si="14"/>
         <v>13969686.036646977</v>
       </c>
-      <c r="Y41" s="2">
+      <c r="Y41" s="3">
         <f t="shared" si="15"/>
         <v>3737.6043178280624</v>
       </c>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2">
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3">
         <f t="shared" si="16"/>
         <v>4.1420684830000001</v>
       </c>
-      <c r="AC41" s="2">
+      <c r="AC41" s="3">
         <f t="shared" si="9"/>
         <v>-2.7555811060000002</v>
       </c>
-      <c r="AD41" s="2">
+      <c r="AD41" s="3">
         <f t="shared" si="10"/>
         <v>13.844604608000001</v>
       </c>
-      <c r="AE41" s="2">
+      <c r="AE41" s="3">
         <f t="shared" si="17"/>
         <v>-109031.72565145828</v>
       </c>
@@ -3525,6 +3552,72 @@
       <c r="AE44">
         <f t="shared" si="17"/>
         <v>122615.38828543811</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>-3531.94634766229</v>
+      </c>
+      <c r="C53">
+        <v>5852.8489434941303</v>
+      </c>
+      <c r="D53">
+        <v>-1.4893779718407E-3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="G53" s="4">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>30.691480120000001</v>
+      </c>
+      <c r="B54">
+        <v>-3502.8717949997399</v>
+      </c>
+      <c r="C54">
+        <v>5865.0782178873596</v>
+      </c>
+      <c r="D54">
+        <v>232.46072917791801</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="F54">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G54">
+        <v>7.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Fixed bug in Ancas(removed old function declaretion) -Removed prints
</commit_message>
<xml_diff>
--- a/Test Data/test.xlsx
+++ b/Test Data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halel\Desktop\פרויקט גמר\test\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B175C9-B1ED-47DC-ACFC-4418597C94CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17F11D5-FCCD-4D3B-BAB2-B0B507F41779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>r1x</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>ancas points</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -488,7 +497,7 @@
   <dimension ref="A1:AE54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +551,15 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
       <c r="S1" t="s">
         <v>18</v>
       </c>
@@ -622,6 +640,16 @@
       <c r="O2">
         <v>126168.7616</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R2">
+        <f>(Q2-P2)/2*COS(PI()*(15-S2+1)/15)+(Q2+P2)/2</f>
+        <v>0</v>
+      </c>
       <c r="S2">
         <v>1</v>
       </c>
@@ -711,6 +739,16 @@
       <c r="O3">
         <v>137211.5055</v>
       </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R17" si="1">(Q3-P3)/2*COS(PI()*(15-S3+1)/15)+(Q3+P3)/2</f>
+        <v>30.691480124178042</v>
+      </c>
       <c r="S3">
         <f>S2+1</f>
         <v>2</v>
@@ -719,27 +757,27 @@
         <v>30.691480120000001</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U17" si="1">B3-H3</f>
+        <f t="shared" ref="U3:U17" si="2">B3-H3</f>
         <v>-1684.8373139999999</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V17" si="2">C3-I3</f>
+        <f t="shared" ref="V3:V17" si="3">C3-I3</f>
         <v>680.39439000000039</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W17" si="3">D3-J3</f>
+        <f t="shared" ref="W3:W17" si="4">D3-J3</f>
         <v>-4477.7539732000005</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X17" si="4">U3*U3+V3*V3+W3*W3</f>
+        <f t="shared" ref="X3:X17" si="5">U3*U3+V3*V3+W3*W3</f>
         <v>23351893.945098598</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y17" si="5">SQRT(X3)</f>
+        <f t="shared" ref="Y3:Y17" si="6">SQRT(X3)</f>
         <v>4832.3797393311916</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB17" si="6">E3-K3</f>
+        <f t="shared" ref="AB3:AB17" si="7">E3-K3</f>
         <v>-3.7728800250000001</v>
       </c>
       <c r="AC3">
@@ -751,7 +789,7 @@
         <v>-13.463346827999999</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE17" si="7">2*( U3*AB3+V3*AC3+W3*AD3)</f>
+        <f t="shared" ref="AE3:AE17" si="8">2*( U3*AB3+V3*AC3+W3*AD3)</f>
         <v>137211.50547442568</v>
       </c>
     </row>
@@ -801,35 +839,45 @@
       <c r="O4">
         <v>165920.72229999999</v>
       </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>121.42455554122466</v>
+      </c>
       <c r="S4">
-        <f t="shared" ref="S4:S17" si="8">S3+1</f>
+        <f t="shared" ref="S4:S17" si="9">S3+1</f>
         <v>3</v>
       </c>
       <c r="T4">
         <v>121.4245555</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2017.7832090000002</v>
       </c>
       <c r="V4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>937.97476900000038</v>
       </c>
       <c r="W4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5674.4848453000004</v>
       </c>
       <c r="X4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37151024.005342312</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6095.163985106743</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.5599233100000003</v>
       </c>
       <c r="AC4">
@@ -841,7 +889,7 @@
         <v>-12.893321665</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>165920.72230075946</v>
       </c>
     </row>
@@ -891,35 +939,45 @@
       <c r="O5">
         <v>197655.0956</v>
       </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>268.23375546981379</v>
+      </c>
       <c r="S5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="T5">
         <v>268.23375540000001</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2510.6806040000001</v>
       </c>
       <c r="V5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1331.9515710000001</v>
       </c>
       <c r="W5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7483.45262</v>
       </c>
       <c r="X5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64079675.198576033</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8004.9781510367684</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.1400623519999997</v>
       </c>
       <c r="AC5">
@@ -931,7 +989,7 @@
         <v>-11.695539384</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>197655.09559769064</v>
       </c>
     </row>
@@ -981,35 +1039,45 @@
       <c r="O6">
         <v>207088.99179999999</v>
       </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>464.70281340436509</v>
+      </c>
       <c r="S6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="T6">
         <v>464.70281340000003</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3062.1135128000001</v>
       </c>
       <c r="V6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1799.4238669999995</v>
       </c>
       <c r="W6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-9584.9625859999996</v>
       </c>
       <c r="X6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>104485973.19342138</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10221.838053570473</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.451394107</v>
       </c>
       <c r="AC6">
@@ -1021,7 +1089,7 @@
         <v>-9.6118941870000008</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>207088.9918296675</v>
       </c>
     </row>
@@ -1071,35 +1139,45 @@
       <c r="O7">
         <v>166837.81340000001</v>
       </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>702.24508875000038</v>
+      </c>
       <c r="S7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="T7">
         <v>702.2450887</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3530.5370991999998</v>
       </c>
       <c r="V7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2245.4459970000003</v>
       </c>
       <c r="W7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-11508.906363</v>
       </c>
       <c r="X7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149961645.60657275</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12245.882802255326</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.470273712</v>
       </c>
       <c r="AC7">
@@ -1111,7 +1189,7 @@
         <v>-6.4923285059999998</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>166837.81338180942</v>
       </c>
     </row>
@@ -1161,37 +1239,47 @@
       <c r="O8">
         <v>67753.860520000002</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>970.47884421981371</v>
+      </c>
       <c r="S8" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="T8" s="1">
         <v>970.47884409999995</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3762.6945269999997</v>
       </c>
       <c r="V8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2558.2957262</v>
       </c>
       <c r="W8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-12715.764122</v>
       </c>
       <c r="X8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>182393404.33255136</v>
       </c>
       <c r="Y8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13505.310227186614</v>
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.24863004599999972</v>
       </c>
       <c r="AC8" s="1">
@@ -1203,7 +1291,7 @@
         <v>-2.4388795320000001</v>
       </c>
       <c r="AE8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>67753.86051418657</v>
       </c>
     </row>
@@ -1253,37 +1341,47 @@
       <c r="O9">
         <v>-63270.349900000001</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>1257.6809775714114</v>
+      </c>
       <c r="S9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="T9" s="1">
         <v>1257.680977</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3642.6177499999999</v>
       </c>
       <c r="V9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2641.7748595000003</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-12759.933706</v>
       </c>
       <c r="X9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>183063546.66241619</v>
       </c>
       <c r="Y9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13530.097806831116</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0774567119999996</v>
       </c>
       <c r="AC9" s="1">
@@ -1295,7 +1393,7 @@
         <v>2.1350048670000001</v>
       </c>
       <c r="AE9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-63270.349912888094</v>
       </c>
     </row>
@@ -1345,35 +1443,45 @@
       <c r="O10">
         <v>-171190.9276</v>
       </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>1551.299377428589</v>
+      </c>
       <c r="S10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="T10">
         <v>1551.299377</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3139.4028903900003</v>
       </c>
       <c r="V10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2451.3032870000002</v>
       </c>
       <c r="W10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-11467.424074</v>
       </c>
       <c r="X10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147366553.20600086</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12139.462640743241</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.3201524759999996</v>
       </c>
       <c r="AC10">
@@ -1385,7 +1493,7 @@
         <v>6.5919548680000002</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-171190.9276049356</v>
       </c>
     </row>
@@ -1435,35 +1543,45 @@
       <c r="O11">
         <v>-208689.06520000001</v>
       </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>1838.5015107801864</v>
+      </c>
       <c r="S11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="T11">
         <v>1838.5015109999999</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2325.1241170000003</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2013.8817759999997</v>
       </c>
       <c r="W11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-9022.9067049999994</v>
       </c>
       <c r="X11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90874767.374293894</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9532.8257811781023</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3025728660000002</v>
       </c>
       <c r="AC11">
@@ -1475,7 +1593,7 @@
         <v>10.286643285</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-208689.06521712933</v>
       </c>
     </row>
@@ -1525,37 +1643,47 @@
       <c r="O12">
         <v>-168807.85130000001</v>
       </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R12">
+        <f>(Q12-P12)/2*COS(PI()*(15-S12+1)/15)+(Q12+P12)/2</f>
+        <v>2106.7352662500002</v>
+      </c>
       <c r="S12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="T12" s="1">
         <v>2106.7352660000001</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1348.9359050000003</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1418.8999930000009</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5902.8642139999993</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38676711.194855399</v>
       </c>
       <c r="Y12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6219.0603144571123</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.9221611049999998</v>
       </c>
       <c r="AC12" s="1">
@@ -1567,7 +1695,7 @@
         <v>12.803499988999999</v>
       </c>
       <c r="AE12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-168807.85134215749</v>
       </c>
     </row>
@@ -1617,37 +1745,47 @@
       <c r="O13">
         <v>-83403.31581</v>
       </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>2344.2775415956357</v>
+      </c>
       <c r="S13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="T13" s="1">
         <v>2344.2775409999999</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-380.70871299999999</v>
       </c>
       <c r="V13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>783.81806299999971</v>
       </c>
       <c r="W13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2690.1918674999997</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7996442.1640023245</v>
       </c>
       <c r="Y13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2827.7981123132404</v>
       </c>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1820954310000005</v>
       </c>
       <c r="AC13" s="1">
@@ -1659,7 +1797,7 @@
         <v>14.086752273</v>
       </c>
       <c r="AE13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-83403.315822714969</v>
       </c>
     </row>
@@ -1709,37 +1847,47 @@
       <c r="O14">
         <v>5893.5407290000003</v>
       </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>2540.7465995301864</v>
+      </c>
       <c r="S14" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="T14" s="2">
         <v>2540.7465990000001</v>
       </c>
       <c r="U14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>443.66045500000018</v>
       </c>
       <c r="V14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>214.36265999999978</v>
       </c>
       <c r="W14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119.85848899999996</v>
       </c>
       <c r="X14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>257152.00671844583</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>507.10157436005443</v>
       </c>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1758960539999999</v>
       </c>
       <c r="AC14" s="1">
@@ -1751,7 +1899,7 @@
         <v>14.403409721999999</v>
       </c>
       <c r="AE14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5893.5407201474391</v>
       </c>
     </row>
@@ -1801,35 +1949,45 @@
       <c r="O15">
         <v>72844.87586</v>
       </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>2687.5557994587753</v>
+      </c>
       <c r="S15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="T15">
         <v>2687.5557990000002</v>
       </c>
       <c r="U15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1048.0709609999999</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-219.70895700000074</v>
       </c>
       <c r="W15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2223.2467085000003</v>
       </c>
       <c r="X15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6089550.6919335769</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2467.7014997632064</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.0394553880000004</v>
       </c>
       <c r="AC15">
@@ -1841,7 +1999,7 @@
         <v>14.186713904000001</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>72844.875863265683</v>
       </c>
     </row>
@@ -1891,35 +2049,45 @@
       <c r="O16">
         <v>110751.5496</v>
       </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>2778.2888748758223</v>
+      </c>
       <c r="S16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="T16">
         <v>2778.2888750000002</v>
       </c>
       <c r="U16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1408.5793189999999</v>
       </c>
       <c r="V16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-485.84599900000012</v>
       </c>
       <c r="W16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3496.7610317999997</v>
       </c>
       <c r="X16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14447479.74617381</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3800.984049713154</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.9002295829999998</v>
       </c>
       <c r="AC16">
@@ -1931,7 +2099,7 @@
         <v>13.860759935000001</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>110751.54964042228</v>
       </c>
     </row>
@@ -1981,35 +2149,45 @@
       <c r="O17">
         <v>122615.38830000001</v>
       </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>2808.9803550000001</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>2808.9803550000001</v>
+      </c>
       <c r="S17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="T17">
         <v>2808.9803550000001</v>
       </c>
       <c r="U17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1527.431497</v>
       </c>
       <c r="V17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-574.88248199999998</v>
       </c>
       <c r="W17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3920.0189278900002</v>
       </c>
       <c r="X17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18030085.241154008</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4246.1847865058826</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8439319909999998</v>
       </c>
       <c r="AC17">
@@ -2021,7 +2199,7 @@
         <v>13.71794336</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>122615.38828543811</v>
       </c>
     </row>
@@ -2044,6 +2222,11 @@
         <v>7954</v>
       </c>
     </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>2508.3142275281102</v>
+      </c>
+    </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
@@ -2194,11 +2377,11 @@
         <v>-3.8363229269999999</v>
       </c>
       <c r="AC28">
-        <f t="shared" ref="AC28:AC44" si="9">F28-L28</f>
+        <f t="shared" ref="AC28:AC44" si="10">F28-L28</f>
         <v>2.9126198830000001</v>
       </c>
       <c r="AD28">
-        <f t="shared" ref="AD28:AD44" si="10">G28-M28</f>
+        <f t="shared" ref="AD28:AD44" si="11">G28-M28</f>
         <v>-13.625315727</v>
       </c>
       <c r="AE28">
@@ -2254,39 +2437,39 @@
         <v>175.56127219999999</v>
       </c>
       <c r="U29">
-        <f t="shared" ref="U29:U44" si="11">B29-H29</f>
+        <f t="shared" ref="U29:U44" si="12">B29-H29</f>
         <v>-2206.6533099999997</v>
       </c>
       <c r="V29">
-        <f t="shared" ref="V29:V44" si="12">C29-I29</f>
+        <f t="shared" ref="V29:V44" si="13">C29-I29</f>
         <v>1086.9442620000009</v>
       </c>
       <c r="W29">
-        <f t="shared" ref="W29:W44" si="13">D29-J29</f>
+        <f t="shared" ref="W29:W44" si="14">D29-J29</f>
         <v>-6361.7824250000003</v>
       </c>
       <c r="X29">
-        <f t="shared" ref="X29:X44" si="14">U29*U29+V29*V29+W29*W29</f>
+        <f t="shared" ref="X29:X44" si="15">U29*U29+V29*V29+W29*W29</f>
         <v>46523042.28226757</v>
       </c>
       <c r="Y29">
-        <f t="shared" ref="Y29:Y44" si="15">SQRT(X29)</f>
+        <f t="shared" ref="Y29:Y44" si="16">SQRT(X29)</f>
         <v>6820.7801813478472</v>
       </c>
       <c r="AB29">
-        <f t="shared" ref="AB29:AB44" si="16">E29-K29</f>
+        <f t="shared" ref="AB29:AB44" si="17">E29-K29</f>
         <v>-3.4155029780000001</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.714690933</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-12.490130657</v>
       </c>
       <c r="AE29">
-        <f t="shared" ref="AE29:AE44" si="17">2*( U29*AB29+V29*AC29+W29*AD29)</f>
+        <f t="shared" ref="AE29:AE44" si="18">2*( U29*AB29+V29*AC29+W29*AD29)</f>
         <v>179894.08476820527</v>
       </c>
     </row>
@@ -2331,46 +2514,46 @@
         <v>6.9972171599999999</v>
       </c>
       <c r="S30">
-        <f t="shared" ref="S30:S44" si="18">S29+1</f>
+        <f t="shared" ref="S30:S44" si="19">S29+1</f>
         <v>3</v>
       </c>
       <c r="T30">
         <v>351.12254430000002</v>
       </c>
       <c r="U30">
+        <f t="shared" si="12"/>
+        <v>-2759.7600709999997</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="13"/>
+        <v>1538.6095549999995</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="14"/>
+        <v>-8419.7155079999993</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="15"/>
+        <v>80875204.247878894</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="16"/>
+        <v>8993.064230165317</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="17"/>
+        <v>-2.8656949639999998</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="10"/>
+        <v>2.4146397369999999</v>
+      </c>
+      <c r="AD30">
         <f t="shared" si="11"/>
-        <v>-2759.7600709999997</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="12"/>
-        <v>1538.6095549999995</v>
-      </c>
-      <c r="W30">
-        <f t="shared" si="13"/>
-        <v>-8419.7155079999993</v>
-      </c>
-      <c r="X30">
-        <f t="shared" si="14"/>
-        <v>80875204.247878894</v>
-      </c>
-      <c r="Y30">
-        <f t="shared" si="15"/>
-        <v>8993.064230165317</v>
-      </c>
-      <c r="AB30">
-        <f t="shared" si="16"/>
-        <v>-2.8656949639999998</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="9"/>
-        <v>2.4146397369999999</v>
-      </c>
-      <c r="AD30">
-        <f t="shared" si="10"/>
         <v>-10.879206575</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>206447.28524561384</v>
       </c>
     </row>
@@ -2415,46 +2598,46 @@
         <v>6.298317108</v>
       </c>
       <c r="S31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="T31">
         <v>526.68381650000003</v>
       </c>
       <c r="U31">
+        <f t="shared" si="12"/>
+        <v>-3206.5911301000001</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="13"/>
+        <v>1929.5524609999998</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="14"/>
+        <v>-10157.466123</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="15"/>
+        <v>117179517.41527981</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="16"/>
+        <v>10824.948841231528</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="17"/>
+        <v>-2.2087752649999999</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="10"/>
+        <v>2.0253251030000001</v>
+      </c>
+      <c r="AD31">
         <f t="shared" si="11"/>
-        <v>-3206.5911301000001</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="12"/>
-        <v>1929.5524609999998</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="13"/>
-        <v>-10157.466123</v>
-      </c>
-      <c r="X31">
-        <f t="shared" si="14"/>
-        <v>117179517.41527981</v>
-      </c>
-      <c r="Y31">
-        <f t="shared" si="15"/>
-        <v>10824.948841231528</v>
-      </c>
-      <c r="AB31">
-        <f t="shared" si="16"/>
-        <v>-2.2087752649999999</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" si="9"/>
-        <v>2.0253251030000001</v>
-      </c>
-      <c r="AD31">
-        <f t="shared" si="10"/>
         <v>-8.8542472330000006</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>201854.65304763199</v>
       </c>
     </row>
@@ -2499,46 +2682,46 @@
         <v>5.358770539</v>
       </c>
       <c r="S32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
       <c r="T32">
         <v>702.2450887</v>
       </c>
       <c r="U32">
+        <f t="shared" si="12"/>
+        <v>-3530.5370991999998</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="13"/>
+        <v>2245.4459970000003</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="14"/>
+        <v>-11508.906363</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="15"/>
+        <v>149961645.60657275</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="16"/>
+        <v>12245.882802255326</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="17"/>
+        <v>-1.470273712</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="10"/>
+        <v>1.5624735379999999</v>
+      </c>
+      <c r="AD32">
         <f t="shared" si="11"/>
-        <v>-3530.5370991999998</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="12"/>
-        <v>2245.4459970000003</v>
-      </c>
-      <c r="W32">
-        <f t="shared" si="13"/>
-        <v>-11508.906363</v>
-      </c>
-      <c r="X32">
-        <f t="shared" si="14"/>
-        <v>149961645.60657275</v>
-      </c>
-      <c r="Y32">
-        <f t="shared" si="15"/>
-        <v>12245.882802255326</v>
-      </c>
-      <c r="AB32">
-        <f t="shared" si="16"/>
-        <v>-1.470273712</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="9"/>
-        <v>1.5624735379999999</v>
-      </c>
-      <c r="AD32">
-        <f t="shared" si="10"/>
         <v>-6.4923285059999998</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>166837.81338180942</v>
       </c>
     </row>
@@ -2583,46 +2766,46 @@
         <v>4.2151120549999996</v>
       </c>
       <c r="S33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
       <c r="T33">
         <v>877.80636079999999</v>
       </c>
       <c r="U33">
+        <f t="shared" si="12"/>
+        <v>-3719.7096872000002</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="13"/>
+        <v>2474.9151671</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="14"/>
+        <v>-12422.573013000001</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="15"/>
+        <v>174281765.50470707</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="16"/>
+        <v>13201.581931901459</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="17"/>
+        <v>-0.6782653569999999</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="10"/>
+        <v>1.0438663840000002</v>
+      </c>
+      <c r="AD33">
         <f t="shared" si="11"/>
-        <v>-3719.7096872000002</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="12"/>
-        <v>2474.9151671</v>
-      </c>
-      <c r="W33">
-        <f t="shared" si="13"/>
-        <v>-12422.573013000001</v>
-      </c>
-      <c r="X33">
-        <f t="shared" si="14"/>
-        <v>174281765.50470707</v>
-      </c>
-      <c r="Y33">
-        <f t="shared" si="15"/>
-        <v>13201.581931901459</v>
-      </c>
-      <c r="AB33">
-        <f t="shared" si="16"/>
-        <v>-0.6782653569999999</v>
-      </c>
-      <c r="AC33">
-        <f t="shared" si="9"/>
-        <v>1.0438663840000002</v>
-      </c>
-      <c r="AD33">
-        <f t="shared" si="10"/>
         <v>-3.8829021209999999</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>106684.13213113512</v>
       </c>
     </row>
@@ -2667,46 +2850,46 @@
         <v>2.911353284</v>
       </c>
       <c r="S34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
       <c r="T34">
         <v>1053.3676330000001</v>
       </c>
       <c r="U34">
+        <f t="shared" si="12"/>
+        <v>-3767.2951560000001</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="13"/>
+        <v>2609.8348288000002</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="14"/>
+        <v>-12863.553046000001</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="15"/>
+        <v>186474747.59329447</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="16"/>
+        <v>13655.575696150436</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="17"/>
+        <v>0.13768411999999985</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="10"/>
+        <v>0.48864122300000012</v>
+      </c>
+      <c r="AD34">
         <f t="shared" si="11"/>
-        <v>-3767.2951560000001</v>
-      </c>
-      <c r="V34">
-        <f t="shared" si="12"/>
-        <v>2609.8348288000002</v>
-      </c>
-      <c r="W34">
-        <f t="shared" si="13"/>
-        <v>-12863.553046000001</v>
-      </c>
-      <c r="X34">
-        <f t="shared" si="14"/>
-        <v>186474747.59329447</v>
-      </c>
-      <c r="Y34">
-        <f t="shared" si="15"/>
-        <v>13655.575696150436</v>
-      </c>
-      <c r="AB34">
-        <f t="shared" si="16"/>
-        <v>0.13768411999999985</v>
-      </c>
-      <c r="AC34">
-        <f t="shared" si="9"/>
-        <v>0.48864122300000012</v>
-      </c>
-      <c r="AD34">
-        <f t="shared" si="10"/>
         <v>-1.124477763</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30442.711035273245</v>
       </c>
     </row>
@@ -2751,46 +2934,46 @@
         <v>1.497209743</v>
       </c>
       <c r="S35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="T35">
         <v>1228.928905</v>
       </c>
       <c r="U35">
+        <f t="shared" si="12"/>
+        <v>-3671.730626</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="13"/>
+        <v>2645.5179923999999</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="14"/>
+        <v>-12814.767297999999</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="15"/>
+        <v>184698632.13990867</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="16"/>
+        <v>13590.387490425306</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="17"/>
+        <v>0.94747878800000018</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="10"/>
+        <v>-8.3257356999999921E-2</v>
+      </c>
+      <c r="AD35">
         <f t="shared" si="11"/>
-        <v>-3671.730626</v>
-      </c>
-      <c r="V35">
-        <f t="shared" si="12"/>
-        <v>2645.5179923999999</v>
-      </c>
-      <c r="W35">
-        <f t="shared" si="13"/>
-        <v>-12814.767297999999</v>
-      </c>
-      <c r="X35">
-        <f t="shared" si="14"/>
-        <v>184698632.13990867</v>
-      </c>
-      <c r="Y35">
-        <f t="shared" si="15"/>
-        <v>13590.387490425306</v>
-      </c>
-      <c r="AB35">
-        <f t="shared" si="16"/>
-        <v>0.94747878800000018</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="9"/>
-        <v>-8.3257356999999921E-2</v>
-      </c>
-      <c r="AD35">
-        <f t="shared" si="10"/>
         <v>1.6788951920000001</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-50427.593845078321</v>
       </c>
     </row>
@@ -2835,46 +3018,46 @@
         <v>2.6245290000000001E-2</v>
       </c>
       <c r="S36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="T36">
         <v>1404.4901769999999</v>
       </c>
       <c r="U36">
+        <f t="shared" si="12"/>
+        <v>-3436.7195211999997</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="13"/>
+        <v>2580.8188243999998</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="14"/>
+        <v>-12277.624659999999</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="15"/>
+        <v>169211734.16361466</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="16"/>
+        <v>13008.141072559702</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="17"/>
+        <v>1.7213671110000002</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="10"/>
+        <v>-0.65150668099999987</v>
+      </c>
+      <c r="AD36">
         <f t="shared" si="11"/>
-        <v>-3436.7195211999997</v>
-      </c>
-      <c r="V36">
-        <f t="shared" si="12"/>
-        <v>2580.8188243999998</v>
-      </c>
-      <c r="W36">
-        <f t="shared" si="13"/>
-        <v>-12277.624659999999</v>
-      </c>
-      <c r="X36">
-        <f t="shared" si="14"/>
-        <v>169211734.16361466</v>
-      </c>
-      <c r="Y36">
-        <f t="shared" si="15"/>
-        <v>13008.141072559702</v>
-      </c>
-      <c r="AB36">
-        <f t="shared" si="16"/>
-        <v>1.7213671110000002</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="9"/>
-        <v>-0.65150668099999987</v>
-      </c>
-      <c r="AD36">
-        <f t="shared" si="10"/>
         <v>4.4212671370000001</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-123759.87017950263</v>
       </c>
     </row>
@@ -2919,46 +3102,46 @@
         <v>-1.446006065</v>
       </c>
       <c r="S37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="T37">
         <v>1580.0514499999999</v>
       </c>
       <c r="U37">
+        <f t="shared" si="12"/>
+        <v>-3071.0976321200001</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="13"/>
+        <v>2418.1650280000003</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="14"/>
+        <v>-11272.030193999999</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="15"/>
+        <v>142337827.46310297</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="16"/>
+        <v>11930.541792521535</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="17"/>
+        <v>2.4307749869999995</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="10"/>
+        <v>-1.1957921469999997</v>
+      </c>
+      <c r="AD37">
         <f t="shared" si="11"/>
-        <v>-3071.0976321200001</v>
-      </c>
-      <c r="V37">
-        <f t="shared" si="12"/>
-        <v>2418.1650280000003</v>
-      </c>
-      <c r="W37">
-        <f t="shared" si="13"/>
-        <v>-11272.030193999999</v>
-      </c>
-      <c r="X37">
-        <f t="shared" si="14"/>
-        <v>142337827.46310297</v>
-      </c>
-      <c r="Y37">
-        <f t="shared" si="15"/>
-        <v>11930.541792521535</v>
-      </c>
-      <c r="AB37">
-        <f t="shared" si="16"/>
-        <v>2.4307749869999995</v>
-      </c>
-      <c r="AC37">
-        <f t="shared" si="9"/>
-        <v>-1.1957921469999997</v>
-      </c>
-      <c r="AD37">
-        <f t="shared" si="10"/>
         <v>6.9985011859999995</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-178488.17347752291</v>
       </c>
     </row>
@@ -3003,46 +3186,46 @@
         <v>-2.8639214740000001</v>
       </c>
       <c r="S38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
       <c r="T38">
         <v>1755.6127220000001</v>
       </c>
       <c r="U38">
+        <f t="shared" si="12"/>
+        <v>-2588.5523215000003</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="13"/>
+        <v>2163.5188749999998</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="14"/>
+        <v>-9835.7379650000003</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="15"/>
+        <v>108123158.35976666</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="16"/>
+        <v>10398.228616440718</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="17"/>
+        <v>3.049152114</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="10"/>
+        <v>-1.6962456300000004</v>
+      </c>
+      <c r="AD38">
         <f t="shared" si="11"/>
-        <v>-2588.5523215000003</v>
-      </c>
-      <c r="V38">
-        <f t="shared" si="12"/>
-        <v>2163.5188749999998</v>
-      </c>
-      <c r="W38">
-        <f t="shared" si="13"/>
-        <v>-9835.7379650000003</v>
-      </c>
-      <c r="X38">
-        <f t="shared" si="14"/>
-        <v>108123158.35976666</v>
-      </c>
-      <c r="Y38">
-        <f t="shared" si="15"/>
-        <v>10398.228616440718</v>
-      </c>
-      <c r="AB38">
-        <f t="shared" si="16"/>
-        <v>3.049152114</v>
-      </c>
-      <c r="AC38">
-        <f t="shared" si="9"/>
-        <v>-1.6962456300000004</v>
-      </c>
-      <c r="AD38">
-        <f t="shared" si="10"/>
         <v>9.3120182529999997</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-206306.64136449533</v>
       </c>
     </row>
@@ -3087,46 +3270,46 @@
         <v>-4.1736786710000002</v>
       </c>
       <c r="S39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="T39">
         <v>1931.173994</v>
       </c>
       <c r="U39">
+        <f t="shared" si="12"/>
+        <v>-2007.1890260000002</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="13"/>
+        <v>1826.2507889999997</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="14"/>
+        <v>-8023.0482739999998</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="15"/>
+        <v>71733303.337352321</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="16"/>
+        <v>8469.5515428712242</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="17"/>
+        <v>3.5528689379999996</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="10"/>
+        <v>-2.1340123010000003</v>
+      </c>
+      <c r="AD39">
         <f t="shared" si="11"/>
-        <v>-2007.1890260000002</v>
-      </c>
-      <c r="V39">
-        <f t="shared" si="12"/>
-        <v>1826.2507889999997</v>
-      </c>
-      <c r="W39">
-        <f t="shared" si="13"/>
-        <v>-8023.0482739999998</v>
-      </c>
-      <c r="X39">
-        <f t="shared" si="14"/>
-        <v>71733303.337352321</v>
-      </c>
-      <c r="Y39">
-        <f t="shared" si="15"/>
-        <v>8469.5515428712242</v>
-      </c>
-      <c r="AB39">
-        <f t="shared" si="16"/>
-        <v>3.5528689379999996</v>
-      </c>
-      <c r="AC39">
-        <f t="shared" si="9"/>
-        <v>-2.1340123010000003</v>
-      </c>
-      <c r="AD39">
-        <f t="shared" si="10"/>
         <v>11.272509054</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-202936.81100190181</v>
       </c>
     </row>
@@ -3171,48 +3354,48 @@
         <v>-5.3251580430000001</v>
       </c>
       <c r="S40" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>13</v>
       </c>
       <c r="T40" s="3">
         <v>2106.7352660000001</v>
       </c>
       <c r="U40" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1348.9359050000003</v>
       </c>
       <c r="V40" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1418.8999930000009</v>
       </c>
       <c r="W40" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-5902.8642139999993</v>
       </c>
       <c r="X40" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>38676711.194855399</v>
       </c>
       <c r="Y40" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6219.0603144571123</v>
       </c>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
       <c r="AB40" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3.9221611049999998</v>
       </c>
       <c r="AC40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.4919725489999998</v>
       </c>
       <c r="AD40" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.803499988999999</v>
       </c>
       <c r="AE40" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-168807.85134215749</v>
       </c>
     </row>
@@ -3257,48 +3440,48 @@
         <v>-6.2738362280000004</v>
       </c>
       <c r="S41" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>14</v>
       </c>
       <c r="T41" s="3">
         <v>2282.2965380000001</v>
       </c>
       <c r="U41" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-638.78230500000018</v>
       </c>
       <c r="V41" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>956.79749300000003</v>
       </c>
       <c r="W41" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-3556.1470386999999</v>
       </c>
       <c r="X41" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>13969686.036646977</v>
       </c>
       <c r="Y41" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3737.6043178280624</v>
       </c>
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
       <c r="AB41" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.1420684830000001</v>
       </c>
       <c r="AC41" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.7555811060000002</v>
       </c>
       <c r="AD41" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.844604608000001</v>
       </c>
       <c r="AE41" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-109031.72565145828</v>
       </c>
     </row>
@@ -3343,46 +3526,46 @@
         <v>-6.9826082270000001</v>
       </c>
       <c r="S42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>15</v>
       </c>
       <c r="T42">
         <v>2457.85781</v>
       </c>
       <c r="U42">
+        <f t="shared" si="12"/>
+        <v>96.140251000000262</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="13"/>
+        <v>457.53853900000013</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="14"/>
+        <v>-1072.8433649999999</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="15"/>
+        <v>1369577.3483571208</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="16"/>
+        <v>1170.2894293110235</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="17"/>
+        <v>4.2032733960000002</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="10"/>
+        <v>-2.913726289</v>
+      </c>
+      <c r="AD42">
         <f t="shared" si="11"/>
-        <v>96.140251000000262</v>
-      </c>
-      <c r="V42">
-        <f t="shared" si="12"/>
-        <v>457.53853900000013</v>
-      </c>
-      <c r="W42">
-        <f t="shared" si="13"/>
-        <v>-1072.8433649999999</v>
-      </c>
-      <c r="X42">
-        <f t="shared" si="14"/>
-        <v>1369577.3483571208</v>
-      </c>
-      <c r="Y42">
-        <f t="shared" si="15"/>
-        <v>1170.2894293110235</v>
-      </c>
-      <c r="AB42">
-        <f t="shared" si="16"/>
-        <v>4.2032733960000002</v>
-      </c>
-      <c r="AC42">
-        <f t="shared" si="9"/>
-        <v>-2.913726289</v>
-      </c>
-      <c r="AD42">
-        <f t="shared" si="10"/>
         <v>14.354251054999999</v>
       </c>
       <c r="AE42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-32657.802627805773</v>
       </c>
     </row>
@@ -3427,46 +3610,46 @@
         <v>-7.4234320260000004</v>
       </c>
       <c r="S43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="T43">
         <v>2633.4190829999998</v>
       </c>
       <c r="U43">
+        <f t="shared" si="12"/>
+        <v>827.60698900000034</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="13"/>
+        <v>-59.687997999999425</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="14"/>
+        <v>1451.6046459999998</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="15"/>
+        <v>2795652.0336356792</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="16"/>
+        <v>1672.0203448629682</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="17"/>
+        <v>4.1027230039999996</v>
+      </c>
+      <c r="AC43">
+        <f t="shared" si="10"/>
+        <v>-2.9594781640000001</v>
+      </c>
+      <c r="AD43">
         <f t="shared" si="11"/>
-        <v>827.60698900000034</v>
-      </c>
-      <c r="V43">
-        <f t="shared" si="12"/>
-        <v>-59.687997999999425</v>
-      </c>
-      <c r="W43">
-        <f t="shared" si="13"/>
-        <v>1451.6046459999998</v>
-      </c>
-      <c r="X43">
-        <f t="shared" si="14"/>
-        <v>2795652.0336356792</v>
-      </c>
-      <c r="Y43">
-        <f t="shared" si="15"/>
-        <v>1672.0203448629682</v>
-      </c>
-      <c r="AB43">
-        <f t="shared" si="16"/>
-        <v>4.1027230039999996</v>
-      </c>
-      <c r="AC43">
-        <f t="shared" si="9"/>
-        <v>-2.9594781640000001</v>
-      </c>
-      <c r="AD43">
-        <f t="shared" si="10"/>
         <v>14.311667627</v>
       </c>
       <c r="AE43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>48693.941556272686</v>
       </c>
     </row>
@@ -3511,46 +3694,46 @@
         <v>-7.5786623259999999</v>
       </c>
       <c r="S44">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
       <c r="T44">
         <v>2808.9803550000001</v>
       </c>
       <c r="U44">
+        <f t="shared" si="12"/>
+        <v>1527.431497</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="13"/>
+        <v>-574.88248199999998</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="14"/>
+        <v>3920.0189278900002</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="15"/>
+        <v>18030085.241154008</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="16"/>
+        <v>4246.1847865058826</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="17"/>
+        <v>3.8439319909999998</v>
+      </c>
+      <c r="AC44">
+        <f t="shared" si="10"/>
+        <v>-2.8905972550000003</v>
+      </c>
+      <c r="AD44">
         <f t="shared" si="11"/>
-        <v>1527.431497</v>
-      </c>
-      <c r="V44">
-        <f t="shared" si="12"/>
-        <v>-574.88248199999998</v>
-      </c>
-      <c r="W44">
-        <f t="shared" si="13"/>
-        <v>3920.0189278900002</v>
-      </c>
-      <c r="X44">
-        <f t="shared" si="14"/>
-        <v>18030085.241154008</v>
-      </c>
-      <c r="Y44">
-        <f t="shared" si="15"/>
-        <v>4246.1847865058826</v>
-      </c>
-      <c r="AB44">
-        <f t="shared" si="16"/>
-        <v>3.8439319909999998</v>
-      </c>
-      <c r="AC44">
-        <f t="shared" si="9"/>
-        <v>-2.8905972550000003</v>
-      </c>
-      <c r="AD44">
-        <f t="shared" si="10"/>
         <v>13.71794336</v>
       </c>
       <c r="AE44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>122615.38828543811</v>
       </c>
     </row>

</xml_diff>